<commit_message>
Deploying to gh-pages from  @ fffe9eb2c6216407e83220bb7708bb8628368256 🚀
</commit_message>
<xml_diff>
--- a/assets/excel-samples/Personal_Projects_Hobbies_Tracking.xlsx
+++ b/assets/excel-samples/Personal_Projects_Hobbies_Tracking.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\docs\excel-samples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Tabito\Tabito.Web\Tabito.Web.Client\wwwroot\assets\excel-samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E412EBDA-C521-40D5-AD22-92DB289AF1AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66851E6A-635A-4548-9712-9EB00F4C886E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{64250ACF-37B4-4223-B651-1844FDCFD9A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$9</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,19 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="55">
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Company</t>
-  </si>
-  <si>
-    <t>Position</t>
-  </si>
-  <si>
-    <t>Location</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
   <si>
     <t>Status</t>
   </si>
@@ -59,148 +50,124 @@
     <t>Deadline</t>
   </si>
   <si>
-    <t>Follow-up</t>
-  </si>
-  <si>
-    <t>ABC Company</t>
-  </si>
-  <si>
-    <t>Marketing Specialist</t>
-  </si>
-  <si>
-    <t>New York</t>
-  </si>
-  <si>
-    <t>Applied</t>
-  </si>
-  <si>
-    <t>Submitted application</t>
-  </si>
-  <si>
-    <t>XYZ Inc.</t>
-  </si>
-  <si>
-    <t>Software Engineer</t>
-  </si>
-  <si>
-    <t>San Francisco</t>
-  </si>
-  <si>
-    <t>Interview Scheduled</t>
-  </si>
-  <si>
-    <t>Scheduled for phone interview</t>
-  </si>
-  <si>
-    <t>123 Industries</t>
-  </si>
-  <si>
-    <t>Project Manager</t>
-  </si>
-  <si>
-    <t>Chicago</t>
-  </si>
-  <si>
-    <t>Rejected</t>
-  </si>
-  <si>
-    <t>Position filled by another candidate</t>
-  </si>
-  <si>
-    <t>ACME Corporation</t>
-  </si>
-  <si>
-    <t>Graphic Designer</t>
-  </si>
-  <si>
-    <t>Los Angeles</t>
-  </si>
-  <si>
-    <t>Offer Received</t>
-  </si>
-  <si>
-    <t>Received job offer! Decision pending</t>
-  </si>
-  <si>
-    <t>LMN Tech</t>
-  </si>
-  <si>
-    <t>Data Analyst</t>
-  </si>
-  <si>
-    <t>Boston</t>
-  </si>
-  <si>
-    <t>DEF Solutions</t>
-  </si>
-  <si>
-    <t>Sales Representative</t>
-  </si>
-  <si>
-    <t>Seattle</t>
-  </si>
-  <si>
-    <t>Under Review</t>
-  </si>
-  <si>
-    <t>Follow up next week</t>
-  </si>
-  <si>
-    <t>GHI Innovations</t>
-  </si>
-  <si>
-    <t>Product Manager</t>
-  </si>
-  <si>
-    <t>Austin</t>
-  </si>
-  <si>
-    <t>JKL Co.</t>
-  </si>
-  <si>
-    <t>Customer Service Specialist</t>
-  </si>
-  <si>
-    <t>Miami</t>
-  </si>
-  <si>
-    <t>Interview Completed</t>
-  </si>
-  <si>
-    <t>Waiting for feedback</t>
-  </si>
-  <si>
-    <t>Company Contact</t>
-  </si>
-  <si>
-    <t>Management Step</t>
-  </si>
-  <si>
-    <t>John Doe</t>
-  </si>
-  <si>
-    <t>Initial Application</t>
-  </si>
-  <si>
-    <t>Jane Smith</t>
-  </si>
-  <si>
-    <t>Phone Interview</t>
-  </si>
-  <si>
-    <t>Emily Brown</t>
-  </si>
-  <si>
-    <t>Bob Johnson</t>
-  </si>
-  <si>
-    <t>Second Interview</t>
-  </si>
-  <si>
-    <t>Michael Clark</t>
-  </si>
-  <si>
-    <t>Final Interview</t>
+    <t>Date Started</t>
+  </si>
+  <si>
+    <t>Project/Hobby Name</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Next Steps</t>
+  </si>
+  <si>
+    <t>Painting Series</t>
+  </si>
+  <si>
+    <t>Art</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Creating a series of landscape paintings</t>
+  </si>
+  <si>
+    <t>Complete sketches for all paintings</t>
+  </si>
+  <si>
+    <t>Coding Project - Website</t>
+  </si>
+  <si>
+    <t>Technology</t>
+  </si>
+  <si>
+    <t>Planning</t>
+  </si>
+  <si>
+    <t>Developing a personal website using HTML/CSS/JavaScript</t>
+  </si>
+  <si>
+    <t>Finish homepage layout and design</t>
+  </si>
+  <si>
+    <t>Gardening - Vegetable Patch</t>
+  </si>
+  <si>
+    <t>Gardening</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Planted tomatoes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> peppers</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> and herbs in the garden bed</t>
+  </si>
+  <si>
+    <t>Photography Project - Portraits</t>
+  </si>
+  <si>
+    <t>Photography</t>
+  </si>
+  <si>
+    <t>Working on portrait photography series</t>
+  </si>
+  <si>
+    <t>Edit and finalize portraits for exhibition</t>
+  </si>
+  <si>
+    <t>Reading Challenge</t>
+  </si>
+  <si>
+    <t>Personal Development</t>
+  </si>
+  <si>
+    <t>Reading 20 books in the year</t>
+  </si>
+  <si>
+    <t>Read 2 books per month</t>
+  </si>
+  <si>
+    <t>DIY Furniture Project</t>
+  </si>
+  <si>
+    <t>Home Improvement</t>
+  </si>
+  <si>
+    <t>Designing and building a new coffee table for the living room</t>
+  </si>
+  <si>
+    <t>Gather materials and tools needed</t>
+  </si>
+  <si>
+    <t>Cooking - International Cuisine</t>
+  </si>
+  <si>
+    <t>Culinary</t>
+  </si>
+  <si>
+    <t>Mastered making sushi at home</t>
+  </si>
+  <si>
+    <t>Writing - Short Stories</t>
+  </si>
+  <si>
+    <t>Writing</t>
+  </si>
+  <si>
+    <t>Writing a collection of short stories</t>
+  </si>
+  <si>
+    <t>Complete first draft of all stories</t>
   </si>
 </sst>
 </file>
@@ -573,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5502331-A91F-4C83-97E4-FC190D16109E}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection sqref="A1:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,39 +560,33 @@
     <col min="10" max="10" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
       </c>
       <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
-        <v>44</v>
-      </c>
-      <c r="J1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>45108</v>
       </c>
@@ -641,17 +602,14 @@
       <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" s="1">
+        <v>45169</v>
+      </c>
+      <c r="H2" t="s">
         <v>12</v>
       </c>
-      <c r="I2" t="s">
-        <v>46</v>
-      </c>
-      <c r="J2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45112</v>
       </c>
@@ -667,20 +625,14 @@
       <c r="E3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" s="1">
+        <v>45199</v>
+      </c>
+      <c r="H3" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="1">
-        <v>45117</v>
-      </c>
-      <c r="I3" t="s">
-        <v>48</v>
-      </c>
-      <c r="J3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45117</v>
       </c>
@@ -699,37 +651,34 @@
       <c r="F4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45122</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="E5" t="s">
         <v>26</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" s="1">
+        <v>45153</v>
+      </c>
+      <c r="H5" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="1">
-        <v>45127</v>
-      </c>
-      <c r="I5" t="s">
-        <v>50</v>
-      </c>
-      <c r="J5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45127</v>
       </c>
@@ -740,45 +689,42 @@
         <v>29</v>
       </c>
       <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
         <v>30</v>
       </c>
-      <c r="E6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G6" s="1">
+        <v>45291</v>
+      </c>
+      <c r="H6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>45132</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="E7" t="s">
         <v>34</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" s="1">
+        <v>45230</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="1">
-        <v>45137</v>
-      </c>
-      <c r="H7" s="1">
-        <v>45135</v>
-      </c>
-      <c r="I7" t="s">
-        <v>51</v>
-      </c>
-      <c r="J7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>45135</v>
       </c>
@@ -789,13 +735,13 @@
         <v>37</v>
       </c>
       <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
         <v>38</v>
       </c>
-      <c r="E8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>45138</v>
       </c>
@@ -806,19 +752,16 @@
         <v>40</v>
       </c>
       <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s">
         <v>41</v>
       </c>
-      <c r="E9" t="s">
+      <c r="G9" s="1">
+        <v>45199</v>
+      </c>
+      <c r="H9" t="s">
         <v>42</v>
-      </c>
-      <c r="F9" t="s">
-        <v>43</v>
-      </c>
-      <c r="I9" t="s">
-        <v>53</v>
-      </c>
-      <c r="J9" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>